<commit_message>
Fixing the "<1" error
</commit_message>
<xml_diff>
--- a/anchor_index.xlsx
+++ b/anchor_index.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justin/Desktop/thesis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Justin\thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{146048DD-78AA-FD4A-A6C7-ABC492974DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22306426-8D64-4563-A0D6-3FB0438BDAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1000" windowWidth="26900" windowHeight="16440" xr2:uid="{59DDBB14-7F74-8D46-B36C-179774A277BD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{59DDBB14-7F74-8D46-B36C-179774A277BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -342,10 +342,10 @@
     <t>oil</t>
   </si>
   <si>
-    <t>m/02r60</t>
-  </si>
-  <si>
     <t>elevator</t>
+  </si>
+  <si>
+    <t>/m/02r60</t>
   </si>
 </sst>
 </file>
@@ -706,13 +706,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC7C152D-0B58-5D47-AE8A-085862D059B1}">
   <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -720,7 +720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -728,7 +728,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>96</v>
       </c>
@@ -736,7 +736,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>100</v>
       </c>
@@ -744,7 +744,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -752,15 +752,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" t="s">
         <v>102</v>
       </c>
-      <c r="B6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -768,7 +768,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -776,7 +776,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -784,7 +784,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -792,7 +792,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -800,7 +800,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -808,7 +808,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -816,7 +816,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -824,7 +824,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -832,7 +832,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -840,7 +840,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
@@ -848,7 +848,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -856,7 +856,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
@@ -864,7 +864,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
@@ -872,7 +872,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
@@ -880,7 +880,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -888,7 +888,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>38</v>
       </c>
@@ -896,7 +896,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>40</v>
       </c>
@@ -904,7 +904,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>42</v>
       </c>
@@ -912,7 +912,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>44</v>
       </c>
@@ -920,7 +920,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>46</v>
       </c>
@@ -928,7 +928,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>48</v>
       </c>
@@ -936,7 +936,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>50</v>
       </c>
@@ -944,7 +944,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>52</v>
       </c>
@@ -952,7 +952,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>54</v>
       </c>
@@ -960,7 +960,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>56</v>
       </c>
@@ -968,7 +968,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>58</v>
       </c>
@@ -976,7 +976,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>60</v>
       </c>
@@ -984,7 +984,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>62</v>
       </c>
@@ -992,7 +992,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>64</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>66</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>68</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>70</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>74</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>76</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>78</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>80</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>82</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>84</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>86</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>89</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>90</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>92</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>95</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>98</v>
       </c>

</xml_diff>

<commit_message>
I was being dumb
</commit_message>
<xml_diff>
--- a/anchor_index.xlsx
+++ b/anchor_index.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Justin\thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justin/Desktop/thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22306426-8D64-4563-A0D6-3FB0438BDAF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DC8EBE-2E86-FC42-9AAA-1BF8BB257E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{59DDBB14-7F74-8D46-B36C-179774A277BD}"/>
+    <workbookView xWindow="1160" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{59DDBB14-7F74-8D46-B36C-179774A277BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -246,9 +246,6 @@
     <t>bed</t>
   </si>
   <si>
-    <t>/m/F0k1tl</t>
-  </si>
-  <si>
     <t>pen</t>
   </si>
   <si>
@@ -346,6 +343,9 @@
   </si>
   <si>
     <t>/m/02r60</t>
+  </si>
+  <si>
+    <t>/m/0k1tl</t>
   </si>
 </sst>
 </file>
@@ -707,12 +707,12 @@
   <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -720,7 +720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -728,23 +728,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" t="s">
         <v>96</v>
       </c>
-      <c r="B3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" t="s">
         <v>100</v>
       </c>
-      <c r="B4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -752,15 +752,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -768,7 +768,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -776,7 +776,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -784,7 +784,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -792,7 +792,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -800,7 +800,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -808,7 +808,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -816,7 +816,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -824,7 +824,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -832,7 +832,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -840,7 +840,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
@@ -848,7 +848,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -856,7 +856,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
@@ -864,7 +864,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
@@ -872,7 +872,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
@@ -880,7 +880,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -888,7 +888,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>38</v>
       </c>
@@ -896,7 +896,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>40</v>
       </c>
@@ -904,7 +904,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>42</v>
       </c>
@@ -912,7 +912,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>44</v>
       </c>
@@ -920,7 +920,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>46</v>
       </c>
@@ -928,7 +928,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>48</v>
       </c>
@@ -936,7 +936,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>50</v>
       </c>
@@ -944,7 +944,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>52</v>
       </c>
@@ -952,7 +952,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>54</v>
       </c>
@@ -960,7 +960,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>56</v>
       </c>
@@ -968,7 +968,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>58</v>
       </c>
@@ -976,7 +976,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>60</v>
       </c>
@@ -984,7 +984,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>62</v>
       </c>
@@ -992,7 +992,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>64</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>66</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>68</v>
       </c>
@@ -1016,116 +1016,116 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>103</v>
+      </c>
+      <c r="B39" t="s">
         <v>70</v>
       </c>
-      <c r="B39" t="s">
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="B40" t="s">
         <v>72</v>
       </c>
-      <c r="B40" t="s">
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="B41" t="s">
         <v>74</v>
       </c>
-      <c r="B41" t="s">
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="B42" t="s">
         <v>76</v>
       </c>
-      <c r="B42" t="s">
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="B43" t="s">
         <v>78</v>
       </c>
-      <c r="B43" t="s">
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="B44" t="s">
         <v>80</v>
       </c>
-      <c r="B44" t="s">
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="B45" t="s">
         <v>82</v>
       </c>
-      <c r="B45" t="s">
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="B46" t="s">
         <v>84</v>
       </c>
-      <c r="B46" t="s">
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+      <c r="B47" t="s">
         <v>86</v>
       </c>
-      <c r="B47" t="s">
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>89</v>
       </c>
-      <c r="B48" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="B49" t="s">
         <v>90</v>
       </c>
-      <c r="B49" t="s">
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="B50" t="s">
         <v>92</v>
       </c>
-      <c r="B50" t="s">
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>94</v>
+      </c>
+      <c r="B51" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>95</v>
-      </c>
-      <c r="B51" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>97</v>
+      </c>
+      <c r="B52" t="s">
         <v>98</v>
-      </c>
-      <c r="B52" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>